<commit_message>
figures an and scripts complete
</commit_message>
<xml_diff>
--- a/data/summary/18_18_24.xlsx
+++ b/data/summary/18_18_24.xlsx
@@ -163,6 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -172,7 +173,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -540,11 +540,11 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1"/>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
@@ -564,13 +564,13 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="3">
         <v>0.80603100000000005</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="3">
         <v>0.82985399999999998</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="3">
         <v>0.83902200000000005</v>
       </c>
     </row>
@@ -578,13 +578,13 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="3">
         <v>0.80598400000000003</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <v>0.82916999999999996</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="3">
         <v>0.83884300000000001</v>
       </c>
     </row>
@@ -592,13 +592,13 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="3">
         <v>0.80615199999999998</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="3">
         <v>0.82981400000000005</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="3">
         <v>0.83869400000000005</v>
       </c>
     </row>
@@ -606,13 +606,13 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="3">
         <v>0.80586599999999997</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <v>0.82960699999999998</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="3">
         <v>0.83855100000000005</v>
       </c>
     </row>
@@ -620,13 +620,13 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="3">
         <v>0.80594699999999997</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="3">
         <v>0.82935899999999996</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="3">
         <v>0.83867499999999995</v>
       </c>
     </row>
@@ -634,13 +634,13 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="3">
         <v>0.80603800000000003</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="3">
         <v>0.82971399999999995</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="3">
         <v>0.83863799999999999</v>
       </c>
     </row>
@@ -648,13 +648,13 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="3">
         <v>0.80577200000000004</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="3">
         <v>0.82953399999999999</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="3">
         <v>0.83864799999999995</v>
       </c>
     </row>
@@ -662,13 +662,13 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="3">
         <v>0.80578799999999995</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="3">
         <v>0.82967999999999997</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="3">
         <v>0.83866200000000002</v>
       </c>
     </row>
@@ -676,13 +676,13 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="3">
         <v>0.80580200000000002</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="3">
         <v>0.82958500000000002</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="3">
         <v>0.83868799999999999</v>
       </c>
     </row>
@@ -690,13 +690,13 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="3">
         <v>0.80583400000000005</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="3">
         <v>0.82938100000000003</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="3">
         <v>0.83854600000000001</v>
       </c>
     </row>
@@ -704,13 +704,13 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="3">
         <v>0.80584</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="3">
         <v>0.82977900000000004</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="3">
         <v>0.83877400000000002</v>
       </c>
     </row>
@@ -718,13 +718,13 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="3">
         <v>0.80569199999999996</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="3">
         <v>0.82924200000000003</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="3">
         <v>0.83898899999999998</v>
       </c>
     </row>
@@ -732,13 +732,13 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="3">
         <v>0.805952</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="3">
         <v>0.82936299999999996</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="3">
         <v>0.83901099999999995</v>
       </c>
     </row>
@@ -746,13 +746,13 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="3">
         <v>0.805836</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="3">
         <v>0.82977800000000002</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="3">
         <v>0.83850800000000003</v>
       </c>
     </row>
@@ -760,13 +760,13 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="3">
         <v>0.80595000000000006</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="3">
         <v>0.82949600000000001</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="3">
         <v>0.83865800000000001</v>
       </c>
     </row>
@@ -774,13 +774,13 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="3">
         <v>0.80612399999999995</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="3">
         <v>0.82962999999999998</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="3">
         <v>0.83891700000000002</v>
       </c>
     </row>
@@ -788,13 +788,13 @@
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="3">
         <v>0.80596699999999999</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="3">
         <v>0.82969099999999996</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="3">
         <v>0.83894400000000002</v>
       </c>
     </row>
@@ -802,13 +802,13 @@
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="3">
         <v>0.80582100000000001</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="3">
         <v>0.82911199999999996</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="3">
         <v>0.838673</v>
       </c>
     </row>
@@ -816,13 +816,13 @@
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="3">
         <v>0.80593099999999995</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="3">
         <v>0.82920300000000002</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="3">
         <v>0.83848699999999998</v>
       </c>
     </row>
@@ -830,13 +830,13 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="3">
         <v>0.80569000000000002</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="3">
         <v>0.82942000000000005</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="3">
         <v>0.83826800000000001</v>
       </c>
     </row>
@@ -844,13 +844,13 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="3">
         <v>0.80613000000000001</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="3">
         <v>0.82919600000000004</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="3">
         <v>0.83879000000000004</v>
       </c>
     </row>
@@ -858,13 +858,13 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="3">
         <v>0.80604699999999996</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="3">
         <v>0.82933299999999999</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="3">
         <v>0.83870299999999998</v>
       </c>
     </row>
@@ -872,13 +872,13 @@
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="3">
         <v>0.80632499999999996</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="3">
         <v>0.82955999999999996</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="3">
         <v>0.83873500000000001</v>
       </c>
     </row>
@@ -886,13 +886,13 @@
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="3">
         <v>0.80587600000000004</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="3">
         <v>0.82958900000000002</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="3">
         <v>0.83875500000000003</v>
       </c>
     </row>
@@ -900,13 +900,13 @@
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="3">
         <v>0.80604600000000004</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="3">
         <v>0.82931600000000005</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="3">
         <v>0.83867400000000003</v>
       </c>
     </row>
@@ -1005,21 +1005,21 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="2"/>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
@@ -1963,7 +1963,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J27"/>
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1973,21 +1973,21 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="2"/>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
@@ -2931,7 +2931,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J27"/>
+      <selection activeCell="J27" sqref="B3:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2941,21 +2941,21 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="2"/>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
@@ -3899,7 +3899,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J27"/>
+      <selection activeCell="J27" sqref="B3:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3909,21 +3909,21 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="2"/>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
@@ -4874,21 +4874,21 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="2"/>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
new method of analyzing string tension with new and better data
</commit_message>
<xml_diff>
--- a/data/summary/18_18_24.xlsx
+++ b/data/summary/18_18_24.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="avg_plaquette" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -120,15 +120,6 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -163,7 +154,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -529,7 +520,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D27"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -565,13 +556,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>0.80603100000000005</v>
+        <v>0.806002</v>
       </c>
       <c r="C3" s="3">
-        <v>0.82985399999999998</v>
+        <v>0.82964499999999997</v>
       </c>
       <c r="D3" s="3">
-        <v>0.83902200000000005</v>
+        <v>0.83850100000000005</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -579,13 +570,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>0.80598400000000003</v>
+        <v>0.80613599999999996</v>
       </c>
       <c r="C4" s="3">
-        <v>0.82916999999999996</v>
+        <v>0.82960500000000004</v>
       </c>
       <c r="D4" s="3">
-        <v>0.83884300000000001</v>
+        <v>0.83886899999999998</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -593,13 +584,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>0.80615199999999998</v>
+        <v>0.80629600000000001</v>
       </c>
       <c r="C5" s="3">
-        <v>0.82981400000000005</v>
+        <v>0.82964099999999996</v>
       </c>
       <c r="D5" s="3">
-        <v>0.83869400000000005</v>
+        <v>0.83898399999999995</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -607,13 +598,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>0.80586599999999997</v>
+        <v>0.80599299999999996</v>
       </c>
       <c r="C6" s="3">
-        <v>0.82960699999999998</v>
+        <v>0.82981400000000005</v>
       </c>
       <c r="D6" s="3">
-        <v>0.83855100000000005</v>
+        <v>0.83842899999999998</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -621,13 +612,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <v>0.80594699999999997</v>
+        <v>0.80603999999999998</v>
       </c>
       <c r="C7" s="3">
-        <v>0.82935899999999996</v>
+        <v>0.829928</v>
       </c>
       <c r="D7" s="3">
-        <v>0.83867499999999995</v>
+        <v>0.83882999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -635,13 +626,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="3">
-        <v>0.80603800000000003</v>
+        <v>0.80591599999999997</v>
       </c>
       <c r="C8" s="3">
-        <v>0.82971399999999995</v>
+        <v>0.82970699999999997</v>
       </c>
       <c r="D8" s="3">
-        <v>0.83863799999999999</v>
+        <v>0.83867899999999995</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -649,13 +640,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="3">
-        <v>0.80577200000000004</v>
+        <v>0.805898</v>
       </c>
       <c r="C9" s="3">
-        <v>0.82953399999999999</v>
+        <v>0.82960999999999996</v>
       </c>
       <c r="D9" s="3">
-        <v>0.83864799999999995</v>
+        <v>0.83890100000000001</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -663,13 +654,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="3">
-        <v>0.80578799999999995</v>
+        <v>0.80579000000000001</v>
       </c>
       <c r="C10" s="3">
-        <v>0.82967999999999997</v>
+        <v>0.82926999999999995</v>
       </c>
       <c r="D10" s="3">
-        <v>0.83866200000000002</v>
+        <v>0.83859600000000001</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -677,13 +668,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="3">
-        <v>0.80580200000000002</v>
+        <v>0.80601</v>
       </c>
       <c r="C11" s="3">
-        <v>0.82958500000000002</v>
+        <v>0.82937899999999998</v>
       </c>
       <c r="D11" s="3">
-        <v>0.83868799999999999</v>
+        <v>0.83875699999999997</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -691,13 +682,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="3">
-        <v>0.80583400000000005</v>
+        <v>0.806118</v>
       </c>
       <c r="C12" s="3">
-        <v>0.82938100000000003</v>
+        <v>0.82907699999999995</v>
       </c>
       <c r="D12" s="3">
-        <v>0.83854600000000001</v>
+        <v>0.83848299999999998</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -705,13 +696,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="3">
-        <v>0.80584</v>
+        <v>0.80565900000000001</v>
       </c>
       <c r="C13" s="3">
-        <v>0.82977900000000004</v>
+        <v>0.82944600000000002</v>
       </c>
       <c r="D13" s="3">
-        <v>0.83877400000000002</v>
+        <v>0.838673</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -719,13 +710,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="3">
-        <v>0.80569199999999996</v>
+        <v>0.80627899999999997</v>
       </c>
       <c r="C14" s="3">
-        <v>0.82924200000000003</v>
+        <v>0.82898400000000005</v>
       </c>
       <c r="D14" s="3">
-        <v>0.83898899999999998</v>
+        <v>0.83879899999999996</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -733,13 +724,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="3">
-        <v>0.805952</v>
+        <v>0.80579900000000004</v>
       </c>
       <c r="C15" s="3">
-        <v>0.82936299999999996</v>
+        <v>0.82964700000000002</v>
       </c>
       <c r="D15" s="3">
-        <v>0.83901099999999995</v>
+        <v>0.83893200000000001</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -747,13 +738,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="3">
-        <v>0.805836</v>
+        <v>0.80637000000000003</v>
       </c>
       <c r="C16" s="3">
-        <v>0.82977800000000002</v>
+        <v>0.82964300000000002</v>
       </c>
       <c r="D16" s="3">
-        <v>0.83850800000000003</v>
+        <v>0.83899900000000005</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -761,13 +752,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="3">
-        <v>0.80595000000000006</v>
+        <v>0.806006</v>
       </c>
       <c r="C17" s="3">
-        <v>0.82949600000000001</v>
+        <v>0.82958900000000002</v>
       </c>
       <c r="D17" s="3">
-        <v>0.83865800000000001</v>
+        <v>0.83877800000000002</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -775,13 +766,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="3">
-        <v>0.80612399999999995</v>
+        <v>0.80590499999999998</v>
       </c>
       <c r="C18" s="3">
-        <v>0.82962999999999998</v>
+        <v>0.82920300000000002</v>
       </c>
       <c r="D18" s="3">
-        <v>0.83891700000000002</v>
+        <v>0.83910099999999999</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -789,13 +780,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="3">
-        <v>0.80596699999999999</v>
+        <v>0.80616500000000002</v>
       </c>
       <c r="C19" s="3">
-        <v>0.82969099999999996</v>
+        <v>0.82931299999999997</v>
       </c>
       <c r="D19" s="3">
-        <v>0.83894400000000002</v>
+        <v>0.83873299999999995</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -803,13 +794,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="3">
-        <v>0.80582100000000001</v>
+        <v>0.80615800000000004</v>
       </c>
       <c r="C20" s="3">
-        <v>0.82911199999999996</v>
+        <v>0.82961700000000005</v>
       </c>
       <c r="D20" s="3">
-        <v>0.838673</v>
+        <v>0.83862700000000001</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -817,13 +808,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="3">
-        <v>0.80593099999999995</v>
+        <v>0.80569000000000002</v>
       </c>
       <c r="C21" s="3">
-        <v>0.82920300000000002</v>
+        <v>0.829426</v>
       </c>
       <c r="D21" s="3">
-        <v>0.83848699999999998</v>
+        <v>0.83841699999999997</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -831,13 +822,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="3">
-        <v>0.80569000000000002</v>
+        <v>0.80631600000000003</v>
       </c>
       <c r="C22" s="3">
-        <v>0.82942000000000005</v>
+        <v>0.829098</v>
       </c>
       <c r="D22" s="3">
-        <v>0.83826800000000001</v>
+        <v>0.83876799999999996</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -845,13 +836,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="3">
-        <v>0.80613000000000001</v>
+        <v>0.80575200000000002</v>
       </c>
       <c r="C23" s="3">
-        <v>0.82919600000000004</v>
+        <v>0.82983499999999999</v>
       </c>
       <c r="D23" s="3">
-        <v>0.83879000000000004</v>
+        <v>0.83878200000000003</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -859,13 +850,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="3">
-        <v>0.80604699999999996</v>
+        <v>0.80592900000000001</v>
       </c>
       <c r="C24" s="3">
-        <v>0.82933299999999999</v>
+        <v>0.82971399999999995</v>
       </c>
       <c r="D24" s="3">
-        <v>0.83870299999999998</v>
+        <v>0.83840099999999995</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -873,13 +864,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="3">
-        <v>0.80632499999999996</v>
+        <v>0.80609699999999995</v>
       </c>
       <c r="C25" s="3">
-        <v>0.82955999999999996</v>
+        <v>0.82908599999999999</v>
       </c>
       <c r="D25" s="3">
-        <v>0.83873500000000001</v>
+        <v>0.83867000000000003</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -887,13 +878,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="3">
-        <v>0.80587600000000004</v>
+        <v>0.80585899999999999</v>
       </c>
       <c r="C26" s="3">
-        <v>0.82958900000000002</v>
+        <v>0.82959799999999995</v>
       </c>
       <c r="D26" s="3">
-        <v>0.83875500000000003</v>
+        <v>0.83876899999999999</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -901,13 +892,13 @@
         <v>25</v>
       </c>
       <c r="B27" s="3">
-        <v>0.80604600000000004</v>
+        <v>0.80561199999999999</v>
       </c>
       <c r="C27" s="3">
-        <v>0.82931600000000005</v>
+        <v>0.82945800000000003</v>
       </c>
       <c r="D27" s="3">
-        <v>0.83867400000000003</v>
+        <v>0.83876700000000004</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -916,15 +907,15 @@
       </c>
       <c r="B28" s="1">
         <f>AVERAGE(B3:B27)</f>
-        <v>0.8059376399999999</v>
+        <v>0.80599179999999992</v>
       </c>
       <c r="C28" s="1">
         <f>AVERAGE(C3:C27)</f>
-        <v>0.82949623999999988</v>
+        <v>0.82949331999999998</v>
       </c>
       <c r="D28" s="1">
         <f>AVERAGE(D3:D27)</f>
-        <v>0.83871412000000012</v>
+        <v>0.83872979999999997</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -933,15 +924,15 @@
       </c>
       <c r="B29" s="1">
         <f>STDEV(B3:B27)</f>
-        <v>1.5230941095895862E-4</v>
+        <v>2.0982889854990534E-4</v>
       </c>
       <c r="C29" s="1">
         <f>STDEV(C3:C27)</f>
-        <v>2.2072008668597902E-4</v>
+        <v>2.5802918439587406E-4</v>
       </c>
       <c r="D29" s="1">
         <f>STDEV(D3:D27)</f>
-        <v>1.768462891892268E-4</v>
+        <v>1.8674849396983434E-4</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -964,15 +955,15 @@
       </c>
       <c r="B31" s="1">
         <f xml:space="preserve"> B30*B29/5</f>
-        <v>8.5201884490441446E-5</v>
+        <v>1.1737828584881704E-4</v>
       </c>
       <c r="C31" s="1">
         <f xml:space="preserve"> C30*C29/5</f>
-        <v>1.2347081649213666E-4</v>
+        <v>1.4434152575105197E-4</v>
       </c>
       <c r="D31" s="1">
         <f xml:space="preserve"> D30*D29/5</f>
-        <v>9.8927814172453479E-5</v>
+        <v>1.0446710752672534E-4</v>
       </c>
     </row>
   </sheetData>
@@ -993,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B3:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1963,7 +1954,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J27"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3516,7 +3507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>